<commit_message>
finished plots, added percentile rank
</commit_message>
<xml_diff>
--- a/results/by_outcome/full_results_education_observed.xlsx
+++ b/results/by_outcome/full_results_education_observed.xlsx
@@ -597,10 +597,10 @@
         <v>0.324327775849591</v>
       </c>
       <c r="D2" t="n">
-        <v>0.264162236920513</v>
+        <v>0.266347322993771</v>
       </c>
       <c r="E2" t="n">
-        <v>0.38449331477867</v>
+        <v>0.382308228705411</v>
       </c>
       <c r="F2" t="n">
         <v>948</v>
@@ -617,10 +617,10 @@
         <v>0.255441272352262</v>
       </c>
       <c r="D3" t="n">
-        <v>0.224022865519917</v>
+        <v>0.171051162687793</v>
       </c>
       <c r="E3" t="n">
-        <v>0.286859679184607</v>
+        <v>0.339831382016731</v>
       </c>
       <c r="F3" t="n">
         <v>948</v>
@@ -637,10 +637,10 @@
         <v>0.442799701389892</v>
       </c>
       <c r="D4" t="n">
-        <v>0.398893516647061</v>
+        <v>0.390697967538696</v>
       </c>
       <c r="E4" t="n">
-        <v>0.486705886132722</v>
+        <v>0.494901435241087</v>
       </c>
       <c r="F4" t="n">
         <v>948</v>

</xml_diff>